<commit_message>
updated compulsarySchooling to include effect on the parent generation
</commit_message>
<xml_diff>
--- a/estimates/compulsarySchooling.xlsx
+++ b/estimates/compulsarySchooling.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>estimate</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Piopiunik (2014), Table 4 Mother-sons, specification (3)</t>
+  </si>
+  <si>
+    <t>Pischke &amp; von Wachter (2008), Table II, Microzensus Basic Track IV</t>
+  </si>
+  <si>
+    <t>lwage_effect_parents_pw</t>
+  </si>
+  <si>
+    <t>lwage_effect_parents_ks</t>
+  </si>
+  <si>
+    <t>Kamhöfer &amp; Schmitz (2016), Table I, Basic</t>
   </si>
 </sst>
 </file>
@@ -901,7 +913,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,10 +998,39 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="3"/>
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="C4">
+        <v>2.76E-2</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>